<commit_message>
RMarkdown and data cleanup work
</commit_message>
<xml_diff>
--- a/data/Mysis_Pilot.xlsx
+++ b/data/Mysis_Pilot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Cavefish\Projects\Mysis\Pilot\Analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Data Science\Mysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8FB221-EF2F-4ADF-9C7B-4CA90C1DE4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6BDE32-5A0E-46E8-AA9A-300796B34FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1980" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1980" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp_1" sheetId="6" r:id="rId1"/>
@@ -996,6 +996,30 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1019,30 +1043,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3394,14 +3394,14 @@
     <tableColumn id="4" xr3:uid="{8DBEA4F3-2890-48C0-B9FE-5F87B7AF97A9}" name="Group" dataDxfId="6" dataCellStyle="Normal 2"/>
     <tableColumn id="5" xr3:uid="{1C4FF994-E2E4-404E-B359-70CD62C63994}" name="Embryo Output" dataDxfId="5" dataCellStyle="Normal 2"/>
     <tableColumn id="6" xr3:uid="{619AECB7-4437-4A10-963A-65F0D28FF76F}" name="Embryo Quality" dataDxfId="4" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{06C7C799-C086-4223-AA3B-51AFD64D2DB9}" name="Survival Rate" dataDxfId="0" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{06C7C799-C086-4223-AA3B-51AFD64D2DB9}" name="Survival Rate" dataDxfId="3" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4EB776F-AF18-4A2E-A2CD-E5117A11CCA9}" name="Table5" displayName="Table5" ref="A1:E3" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4EB776F-AF18-4A2E-A2CD-E5117A11CCA9}" name="Table5" displayName="Table5" ref="A1:E3" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
   <autoFilter ref="A1:E3" xr:uid="{4285FD4A-F9DE-4FDB-8832-B6BA0A12B52E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6DDE0D8A-E52D-4176-81E0-FCF08002B7A9}" name="Sample ID"/>
@@ -3682,8 +3682,8 @@
   </sheetPr>
   <dimension ref="A1:K794"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8829,7 +8829,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C161" s="59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D161" s="8">
         <v>99</v>
@@ -53201,7 +53201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>

</xml_diff>